<commit_message>
Singular miscoded line in raw data
</commit_message>
<xml_diff>
--- a/data/published/2019_Seale-CarlisleColloffFloweWellsWixtedMickes/Seale-Carlisle_et_al_raw_data.xlsx
+++ b/data/published/2019_Seale-CarlisleColloffFloweWellsWixtedMickes/Seale-Carlisle_et_al_raw_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10503"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sboogert/Psychology/pyWitness/data/published/2019_Seale-CarlisleColloffFloweWellsWixtedMickes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sboogert/Dropbox (Royal Holloway)/Psychology/pyWitness/data/published/2019_Seale-CarlisleColloffFloweWellsWixtedMickes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAED758E-82AB-3846-AC36-32C3E90D7A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCBEB80-1AA1-204D-B468-05A359D17114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30320" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5442,7 +5442,7 @@
         <v>28</v>
       </c>
       <c r="K76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L76">
         <v>80</v>

</xml_diff>